<commit_message>
Java Pgm Completed and Properties file included
</commit_message>
<xml_diff>
--- a/TestData/Chrome/S0130_EditAccount.xlsx
+++ b/TestData/Chrome/S0130_EditAccount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\velsp\eclipse-workspace\FullStackAutomationPgm\TestData\Chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C136B65-2B1E-44A6-927B-649A104DC92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F315F0-DD88-4E57-BF35-933409CC35BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F0947FD-ADC8-4020-92FB-4AE3B928E5BA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>AccountName</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>66953201</t>
+  </si>
+  <si>
+    <t>22953021</t>
+  </si>
+  <si>
+    <t>55452012</t>
   </si>
 </sst>
 </file>
@@ -169,8 +178,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +498,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,8 +572,8 @@
       <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2">
-        <v>66953201</v>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="J2" t="s">
         <v>24</v>
@@ -594,8 +604,8 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="I3">
-        <v>22953021</v>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -626,8 +636,8 @@
       <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="I4">
-        <v>55452012</v>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="J4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Cucumber with TestNG Implementation
</commit_message>
<xml_diff>
--- a/TestData/Chrome/S0130_EditAccount.xlsx
+++ b/TestData/Chrome/S0130_EditAccount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\velsp\eclipse-workspace\FullStackAutomationPgm\TestData\Chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F315F0-DD88-4E57-BF35-933409CC35BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948AB693-4E81-4418-9F74-C3CB0DBA32A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F0947FD-ADC8-4020-92FB-4AE3B928E5BA}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>